<commit_message>
Aggiornati data.json e report-checklist.xlsx
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#INFOSERVICEONLINE/INFOSERVICE/FLY/2.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111#INFOSERVICEONLINE/INFOSERVICE/FLY/2.0/report-checklist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DOTNET2019\FSETEST\FSE20Tester\bin\Debug\Pdftest\Seconda pull request\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DOTNET2019\FSETEST\FSE20Tester\bin\Debug\Pdftest\Terza pull request\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C00BB9C0-746B-46BB-ABC1-8D45E79B70F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39739682-A4E2-43FA-A2BE-A12F7AC6CDF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="347" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2154,49 +2154,49 @@
     <t>Erroregestito da un pannello di controllo centralizzato che consenta la gestione e correzione di ogni tipologia di errore prevista.</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.2c8685f071^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>9ac77d7a16c3cfc2</t>
-  </si>
-  <si>
-    <t>2024-05-10T12:28:11Z</t>
-  </si>
-  <si>
-    <t>2024-05-10T12:30:09Z</t>
-  </si>
-  <si>
-    <t>5ea4334f12e42e62</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.b4c19ffdf2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2024-05-10T12:32:06Z</t>
-  </si>
-  <si>
-    <t>e5066719ea34cbd0</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.ff1c4e1e01^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2024-05-10T12:34:10Z</t>
-  </si>
-  <si>
-    <t>8da046774bf7fe65</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.00efd60278^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2024-05-10T12:36:29Z</t>
-  </si>
-  <si>
-    <t>a3e7af4ce0f28e19</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.623935b845^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2024-05-16T07:58:19Z</t>
+  </si>
+  <si>
+    <t>4d918fbc5ea6c2e4</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.a4cca34114^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-05-16T08:05:07Z</t>
+  </si>
+  <si>
+    <t>4364a66ad8fd30a5</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.0aebd64347^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-05-16T08:07:47Z</t>
+  </si>
+  <si>
+    <t>7266eb42fcd3fd64</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.3280aac4ed^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-05-16T08:10:27Z</t>
+  </si>
+  <si>
+    <t>90685ce8dfbf115a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.3713fedaef^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-05-16T08:13:06Z</t>
+  </si>
+  <si>
+    <t>1df3440e30cf0c86</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.e505cf260b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -4176,11 +4176,11 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:T768"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="F66" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <pane xSplit="1" ySplit="9" topLeftCell="D75" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="L71" sqref="L71"/>
+      <selection pane="bottomRight" activeCell="M102" sqref="M102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -5948,16 +5948,16 @@
         <v>395</v>
       </c>
       <c r="F54" s="23">
-        <v>45422</v>
+        <v>45428</v>
       </c>
       <c r="G54" s="24" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="H54" s="24" t="s">
         <v>457</v>
       </c>
       <c r="I54" s="24" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="J54" s="25" t="s">
         <v>84</v>
@@ -5992,7 +5992,7 @@
         <v>61</v>
       </c>
       <c r="F55" s="23">
-        <v>45422</v>
+        <v>45428</v>
       </c>
       <c r="G55" s="47" t="s">
         <v>459</v>
@@ -6036,7 +6036,7 @@
         <v>63</v>
       </c>
       <c r="F56" s="23">
-        <v>45422</v>
+        <v>45428</v>
       </c>
       <c r="G56" s="47" t="s">
         <v>462</v>
@@ -6080,7 +6080,7 @@
         <v>65</v>
       </c>
       <c r="F57" s="23">
-        <v>45422</v>
+        <v>45428</v>
       </c>
       <c r="G57" s="47" t="s">
         <v>465</v>
@@ -7974,7 +7974,7 @@
         <v>333</v>
       </c>
       <c r="F102" s="23">
-        <v>45422</v>
+        <v>45428</v>
       </c>
       <c r="G102" s="24" t="s">
         <v>468</v>

</xml_diff>

<commit_message>
Aggiornata colonna gestione errore
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#INFOSERVICEONLINE/INFOSERVICE/FLY/2.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111#INFOSERVICEONLINE/INFOSERVICE/FLY/2.0/report-checklist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DOTNET2019\FSETEST\FSE20Tester\bin\Debug\Pdftest\Quarta pull request\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DOTNET2019\FSETEST\FSE20Tester\bin\Debug\Pdftest\Chiarimenti certificazione RAD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC393885-4D5F-4967-8F04-8C4A548D5894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF037AA5-F877-4C42-BD5D-F4FD8C7BEA6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="347" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TestCases!$A$9:$T$151</definedName>
   </definedNames>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataChecksum="oXWj5iU3LtnvLpdhFqszSz/X91q3fG5U5zC5TJKtiGw="/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1086" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1086" uniqueCount="464">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -1977,18 +1977,12 @@
     <t>Il software non gestisce  in modo strutturato le informazioni richieste dal test case.</t>
   </si>
   <si>
-    <t>Sezione  "DICOM Object Catalog" non gestita</t>
-  </si>
-  <si>
     <t>Sezione non gestita da applicativo</t>
   </si>
   <si>
     <t>Sezione opzionale non gestita nel CDA</t>
   </si>
   <si>
-    <t>Errore gestito da un pannello di controllo che gestisce tutti gli errori consentendo la soluzione corretta a seconda del caso.</t>
-  </si>
-  <si>
     <t>UNKNOWN_WORKFLOW_ID</t>
   </si>
   <si>
@@ -2151,9 +2145,6 @@
     <t>[ERRORE-40| L'elemento ClinicalDocument/documentationOf/serviceEvent deve contenere l'elemento code e DEVE valorizzare il suo attributo code con uno dei seguenti valori: 'PROG'|'DIR'|'RAD_PROG|'RAD_DIR' ]</t>
   </si>
   <si>
-    <t>Erroregestito da un pannello di controllo centralizzato che consenta la gestione e correzione di ogni tipologia di errore prevista.</t>
-  </si>
-  <si>
     <t>2024-05-16T07:58:19Z</t>
   </si>
   <si>
@@ -2179,6 +2170,12 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.e505cf260b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il sofware non gestisce i tag inerenti l’anamnesi patologica prossima e quella remota </t>
+  </si>
+  <si>
+    <t>Gli errori saranno gestiti tramite un pannello di controllo centralizzato e polimorfico che sarà in grado di riconoscere gli errori, su cui potranno agire gli operatori autorizzati ed effettuare le opportune correzioni, se necessario, reinviando il referto al FSE.</t>
   </si>
 </sst>
 </file>
@@ -2659,6 +2656,9 @@
     <xf numFmtId="164" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2681,9 +2681,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4162,10 +4159,10 @@
   <dimension ref="A1:T768"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="E56" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="J70" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="K57" sqref="K57"/>
+      <selection pane="bottomRight" activeCell="P79" sqref="P79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -4203,14 +4200,14 @@
       <c r="T1" s="15"/>
     </row>
     <row r="2" spans="1:20" ht="21">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="52" t="s">
-        <v>408</v>
-      </c>
-      <c r="D2" s="53"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="53" t="s">
+        <v>406</v>
+      </c>
+      <c r="D2" s="54"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -4228,14 +4225,14 @@
       <c r="T2" s="15"/>
     </row>
     <row r="3" spans="1:20" ht="15.75">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="60" t="s">
+      <c r="B3" s="56"/>
+      <c r="C3" s="61" t="s">
         <v>394</v>
       </c>
-      <c r="D3" s="51"/>
+      <c r="D3" s="52"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -4253,12 +4250,12 @@
       <c r="T3" s="15"/>
     </row>
     <row r="4" spans="1:20" ht="15.75">
-      <c r="A4" s="56"/>
-      <c r="B4" s="57"/>
-      <c r="C4" s="60" t="s">
+      <c r="A4" s="57"/>
+      <c r="B4" s="58"/>
+      <c r="C4" s="61" t="s">
         <v>392</v>
       </c>
-      <c r="D4" s="51"/>
+      <c r="D4" s="52"/>
       <c r="E4" s="4"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
@@ -4277,12 +4274,12 @@
       <c r="T4" s="15"/>
     </row>
     <row r="5" spans="1:20" ht="15.75">
-      <c r="A5" s="58"/>
-      <c r="B5" s="59"/>
-      <c r="C5" s="60" t="s">
+      <c r="A5" s="59"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="61" t="s">
         <v>393</v>
       </c>
-      <c r="D5" s="51"/>
+      <c r="D5" s="52"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -4300,8 +4297,8 @@
       <c r="T5" s="15"/>
     </row>
     <row r="6" spans="1:20">
-      <c r="A6" s="48"/>
-      <c r="B6" s="49"/>
+      <c r="A6" s="49"/>
+      <c r="B6" s="50"/>
       <c r="C6" s="16"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -5936,13 +5933,13 @@
         <v>45428</v>
       </c>
       <c r="G54" s="24" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="H54" s="24" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="I54" s="24" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="J54" s="25" t="s">
         <v>84</v>
@@ -5980,13 +5977,13 @@
         <v>45428</v>
       </c>
       <c r="G55" s="47" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="H55" s="24" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="I55" s="24" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="J55" s="25" t="s">
         <v>84</v>
@@ -6021,9 +6018,9 @@
         <v>63</v>
       </c>
       <c r="F56" s="36"/>
-      <c r="G56" s="61"/>
-      <c r="H56" s="61"/>
-      <c r="I56" s="61"/>
+      <c r="G56" s="48"/>
+      <c r="H56" s="48"/>
+      <c r="I56" s="48"/>
       <c r="J56" s="38" t="s">
         <v>391</v>
       </c>
@@ -6059,9 +6056,9 @@
         <v>65</v>
       </c>
       <c r="F57" s="36"/>
-      <c r="G57" s="61"/>
-      <c r="H57" s="61"/>
-      <c r="I57" s="61"/>
+      <c r="G57" s="48"/>
+      <c r="H57" s="48"/>
+      <c r="I57" s="48"/>
       <c r="J57" s="38" t="s">
         <v>391</v>
       </c>
@@ -6100,13 +6097,13 @@
         <v>45416</v>
       </c>
       <c r="G58" s="47" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="H58" s="47" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="I58" s="47" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="J58" s="25" t="s">
         <v>84</v>
@@ -6119,13 +6116,13 @@
         <v>84</v>
       </c>
       <c r="N58" s="46" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="O58" s="46" t="s">
         <v>84</v>
       </c>
       <c r="P58" s="46" t="s">
-        <v>455</v>
+        <v>463</v>
       </c>
       <c r="Q58" s="25"/>
       <c r="R58" s="26"/>
@@ -6154,13 +6151,13 @@
         <v>45416</v>
       </c>
       <c r="G59" s="24" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="H59" s="47" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="I59" s="47" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="J59" s="25" t="s">
         <v>84</v>
@@ -6173,13 +6170,13 @@
         <v>84</v>
       </c>
       <c r="N59" s="46" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="O59" s="46" t="s">
         <v>84</v>
       </c>
       <c r="P59" s="46" t="s">
-        <v>455</v>
+        <v>463</v>
       </c>
       <c r="Q59" s="25"/>
       <c r="R59" s="26"/>
@@ -6188,7 +6185,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="60" spans="1:20" ht="75">
+    <row r="60" spans="1:20" ht="150">
       <c r="A60" s="20">
         <v>47</v>
       </c>
@@ -6225,7 +6222,7 @@
         <v>84</v>
       </c>
       <c r="P60" s="46" t="s">
-        <v>400</v>
+        <v>463</v>
       </c>
       <c r="Q60" s="25"/>
       <c r="R60" s="26" t="s">
@@ -6236,7 +6233,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="61" spans="1:20" ht="135">
+    <row r="61" spans="1:20" ht="150">
       <c r="A61" s="20">
         <v>75</v>
       </c>
@@ -6256,13 +6253,13 @@
         <v>45416</v>
       </c>
       <c r="G61" s="47" t="s">
+        <v>416</v>
+      </c>
+      <c r="H61" s="47" t="s">
+        <v>417</v>
+      </c>
+      <c r="I61" s="47" t="s">
         <v>418</v>
-      </c>
-      <c r="H61" s="47" t="s">
-        <v>419</v>
-      </c>
-      <c r="I61" s="47" t="s">
-        <v>420</v>
       </c>
       <c r="J61" s="25" t="s">
         <v>84</v>
@@ -6275,13 +6272,13 @@
         <v>84</v>
       </c>
       <c r="N61" s="46" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="O61" s="46" t="s">
         <v>84</v>
       </c>
       <c r="P61" s="46" t="s">
-        <v>455</v>
+        <v>463</v>
       </c>
       <c r="Q61" s="25"/>
       <c r="R61" s="26"/>
@@ -6290,7 +6287,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="62" spans="1:20" ht="120.75" thickBot="1">
+    <row r="62" spans="1:20" ht="150.75" thickBot="1">
       <c r="A62" s="20">
         <v>76</v>
       </c>
@@ -6310,13 +6307,13 @@
         <v>45416</v>
       </c>
       <c r="G62" s="47" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="H62" s="47" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="I62" s="47" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="J62" s="25" t="s">
         <v>84</v>
@@ -6329,13 +6326,13 @@
         <v>84</v>
       </c>
       <c r="N62" s="46" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="O62" s="46" t="s">
         <v>84</v>
       </c>
       <c r="P62" s="46" t="s">
-        <v>455</v>
+        <v>463</v>
       </c>
       <c r="Q62" s="25"/>
       <c r="R62" s="26"/>
@@ -6344,7 +6341,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="63" spans="1:20" ht="105.75" thickBot="1">
+    <row r="63" spans="1:20" ht="150.75" thickBot="1">
       <c r="A63" s="20">
         <v>77</v>
       </c>
@@ -6364,13 +6361,13 @@
         <v>45416</v>
       </c>
       <c r="G63" s="47" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="H63" s="47" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="I63" s="47" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="J63" s="25" t="s">
         <v>84</v>
@@ -6383,13 +6380,13 @@
         <v>84</v>
       </c>
       <c r="N63" s="46" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="O63" s="46" t="s">
         <v>84</v>
       </c>
       <c r="P63" s="46" t="s">
-        <v>455</v>
+        <v>463</v>
       </c>
       <c r="Q63" s="25"/>
       <c r="R63" s="26"/>
@@ -6398,7 +6395,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="64" spans="1:20" ht="105.75" thickBot="1">
+    <row r="64" spans="1:20" ht="150.75" thickBot="1">
       <c r="A64" s="20">
         <v>78</v>
       </c>
@@ -6418,13 +6415,13 @@
         <v>45416</v>
       </c>
       <c r="G64" s="47" t="s">
+        <v>423</v>
+      </c>
+      <c r="H64" s="24" t="s">
+        <v>424</v>
+      </c>
+      <c r="I64" s="47" t="s">
         <v>425</v>
-      </c>
-      <c r="H64" s="24" t="s">
-        <v>426</v>
-      </c>
-      <c r="I64" s="47" t="s">
-        <v>427</v>
       </c>
       <c r="J64" s="25" t="s">
         <v>84</v>
@@ -6437,13 +6434,13 @@
         <v>84</v>
       </c>
       <c r="N64" s="46" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="O64" s="46" t="s">
         <v>84</v>
       </c>
       <c r="P64" s="46" t="s">
-        <v>455</v>
+        <v>463</v>
       </c>
       <c r="Q64" s="25"/>
       <c r="R64" s="26"/>
@@ -6452,7 +6449,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="65" spans="1:20" ht="120.75" thickBot="1">
+    <row r="65" spans="1:20" ht="150.75" thickBot="1">
       <c r="A65" s="20">
         <v>79</v>
       </c>
@@ -6472,13 +6469,13 @@
         <v>45416</v>
       </c>
       <c r="G65" s="47" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="H65" s="47" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="I65" s="47" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="J65" s="25" t="s">
         <v>84</v>
@@ -6491,13 +6488,13 @@
         <v>84</v>
       </c>
       <c r="N65" s="46" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="O65" s="46" t="s">
         <v>84</v>
       </c>
       <c r="P65" s="46" t="s">
-        <v>455</v>
+        <v>463</v>
       </c>
       <c r="Q65" s="25"/>
       <c r="R65" s="26"/>
@@ -6506,7 +6503,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="66" spans="1:20" ht="120.75" thickBot="1">
+    <row r="66" spans="1:20" ht="150.75" thickBot="1">
       <c r="A66" s="20">
         <v>80</v>
       </c>
@@ -6526,13 +6523,13 @@
         <v>45416</v>
       </c>
       <c r="G66" s="47" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="H66" s="47" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="I66" s="47" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="J66" s="25" t="s">
         <v>84</v>
@@ -6545,13 +6542,13 @@
         <v>84</v>
       </c>
       <c r="N66" s="46" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="O66" s="46" t="s">
         <v>84</v>
       </c>
       <c r="P66" s="46" t="s">
-        <v>455</v>
+        <v>463</v>
       </c>
       <c r="Q66" s="25"/>
       <c r="R66" s="26"/>
@@ -6560,7 +6557,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="67" spans="1:20" ht="120.75" thickBot="1">
+    <row r="67" spans="1:20" ht="150.75" thickBot="1">
       <c r="A67" s="20">
         <v>81</v>
       </c>
@@ -6580,13 +6577,13 @@
         <v>45416</v>
       </c>
       <c r="G67" s="47" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="H67" s="47" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="I67" s="47" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="J67" s="25" t="s">
         <v>84</v>
@@ -6599,13 +6596,13 @@
         <v>84</v>
       </c>
       <c r="N67" s="46" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="O67" s="46" t="s">
         <v>84</v>
       </c>
       <c r="P67" s="46" t="s">
-        <v>455</v>
+        <v>463</v>
       </c>
       <c r="Q67" s="25"/>
       <c r="R67" s="26"/>
@@ -6614,7 +6611,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="68" spans="1:20" ht="120.75" thickBot="1">
+    <row r="68" spans="1:20" ht="150.75" thickBot="1">
       <c r="A68" s="20">
         <v>82</v>
       </c>
@@ -6634,13 +6631,13 @@
         <v>45416</v>
       </c>
       <c r="G68" s="47" t="s">
+        <v>430</v>
+      </c>
+      <c r="H68" s="47" t="s">
+        <v>431</v>
+      </c>
+      <c r="I68" s="47" t="s">
         <v>432</v>
-      </c>
-      <c r="H68" s="47" t="s">
-        <v>433</v>
-      </c>
-      <c r="I68" s="47" t="s">
-        <v>434</v>
       </c>
       <c r="J68" s="25" t="s">
         <v>84</v>
@@ -6653,13 +6650,13 @@
         <v>84</v>
       </c>
       <c r="N68" s="46" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="O68" s="46" t="s">
         <v>84</v>
       </c>
       <c r="P68" s="46" t="s">
-        <v>455</v>
+        <v>463</v>
       </c>
       <c r="Q68" s="25"/>
       <c r="R68" s="26"/>
@@ -6668,7 +6665,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="69" spans="1:20" ht="105">
+    <row r="69" spans="1:20" ht="150">
       <c r="A69" s="20">
         <v>83</v>
       </c>
@@ -6688,13 +6685,13 @@
         <v>45416</v>
       </c>
       <c r="G69" s="47" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="H69" s="47" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="I69" s="47" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="J69" s="25" t="s">
         <v>84</v>
@@ -6707,13 +6704,13 @@
         <v>84</v>
       </c>
       <c r="N69" s="46" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="O69" s="46" t="s">
         <v>84</v>
       </c>
       <c r="P69" s="46" t="s">
-        <v>455</v>
+        <v>463</v>
       </c>
       <c r="Q69" s="25"/>
       <c r="R69" s="26"/>
@@ -6722,7 +6719,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="70" spans="1:20" ht="105">
+    <row r="70" spans="1:20" ht="150">
       <c r="A70" s="20">
         <v>84</v>
       </c>
@@ -6742,13 +6739,13 @@
         <v>45416</v>
       </c>
       <c r="G70" s="24" t="s">
+        <v>437</v>
+      </c>
+      <c r="H70" s="24" t="s">
+        <v>438</v>
+      </c>
+      <c r="I70" s="24" t="s">
         <v>439</v>
-      </c>
-      <c r="H70" s="24" t="s">
-        <v>440</v>
-      </c>
-      <c r="I70" s="24" t="s">
-        <v>441</v>
       </c>
       <c r="J70" s="25" t="s">
         <v>84</v>
@@ -6761,13 +6758,13 @@
         <v>84</v>
       </c>
       <c r="N70" s="25" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="O70" s="46" t="s">
         <v>84</v>
       </c>
       <c r="P70" s="46" t="s">
-        <v>455</v>
+        <v>463</v>
       </c>
       <c r="Q70" s="25"/>
       <c r="R70" s="26"/>
@@ -6776,7 +6773,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="71" spans="1:20" ht="120">
+    <row r="71" spans="1:20" ht="150">
       <c r="A71" s="20">
         <v>85</v>
       </c>
@@ -6796,13 +6793,13 @@
         <v>45416</v>
       </c>
       <c r="G71" s="24" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="H71" s="24" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="I71" s="24" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="J71" s="25" t="s">
         <v>84</v>
@@ -6815,13 +6812,13 @@
         <v>84</v>
       </c>
       <c r="N71" s="25" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="O71" s="46" t="s">
         <v>84</v>
       </c>
       <c r="P71" s="46" t="s">
-        <v>455</v>
+        <v>463</v>
       </c>
       <c r="Q71" s="25"/>
       <c r="R71" s="26"/>
@@ -6830,7 +6827,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="72" spans="1:20" ht="120">
+    <row r="72" spans="1:20" ht="150">
       <c r="A72" s="20">
         <v>86</v>
       </c>
@@ -6850,13 +6847,13 @@
         <v>45416</v>
       </c>
       <c r="G72" s="24" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="H72" s="24" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="I72" s="24" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="J72" s="25" t="s">
         <v>84</v>
@@ -6869,13 +6866,13 @@
         <v>84</v>
       </c>
       <c r="N72" s="25" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="O72" s="46" t="s">
         <v>84</v>
       </c>
       <c r="P72" s="46" t="s">
-        <v>400</v>
+        <v>463</v>
       </c>
       <c r="Q72" s="25"/>
       <c r="R72" s="26"/>
@@ -6946,7 +6943,7 @@
         <v>391</v>
       </c>
       <c r="K74" s="43" t="s">
-        <v>397</v>
+        <v>462</v>
       </c>
       <c r="L74" s="38"/>
       <c r="M74" s="38"/>
@@ -6960,7 +6957,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="75" spans="1:20" ht="105">
+    <row r="75" spans="1:20" ht="150">
       <c r="A75" s="20">
         <v>89</v>
       </c>
@@ -6980,13 +6977,13 @@
         <v>45416</v>
       </c>
       <c r="G75" s="24" t="s">
+        <v>444</v>
+      </c>
+      <c r="H75" s="24" t="s">
+        <v>445</v>
+      </c>
+      <c r="I75" s="24" t="s">
         <v>446</v>
-      </c>
-      <c r="H75" s="24" t="s">
-        <v>447</v>
-      </c>
-      <c r="I75" s="24" t="s">
-        <v>448</v>
       </c>
       <c r="J75" s="25" t="s">
         <v>84</v>
@@ -6999,13 +6996,13 @@
         <v>84</v>
       </c>
       <c r="N75" s="25" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="O75" s="46" t="s">
         <v>84</v>
       </c>
       <c r="P75" s="46" t="s">
-        <v>455</v>
+        <v>463</v>
       </c>
       <c r="Q75" s="25"/>
       <c r="R75" s="26"/>
@@ -7038,7 +7035,7 @@
         <v>391</v>
       </c>
       <c r="K76" s="43" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="L76" s="38"/>
       <c r="M76" s="38"/>
@@ -7076,7 +7073,7 @@
         <v>391</v>
       </c>
       <c r="K77" s="43" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="L77" s="38"/>
       <c r="M77" s="38"/>
@@ -7114,7 +7111,7 @@
         <v>391</v>
       </c>
       <c r="K78" s="43" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="L78" s="38"/>
       <c r="M78" s="38"/>
@@ -7128,7 +7125,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="79" spans="1:20" ht="120.75" thickBot="1">
+    <row r="79" spans="1:20" ht="150.75" thickBot="1">
       <c r="A79" s="20">
         <v>93</v>
       </c>
@@ -7148,13 +7145,13 @@
         <v>45416</v>
       </c>
       <c r="G79" s="24" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="H79" s="24" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="I79" s="24" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="J79" s="25" t="s">
         <v>84</v>
@@ -7167,13 +7164,13 @@
         <v>84</v>
       </c>
       <c r="N79" s="25" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="O79" s="46" t="s">
         <v>84</v>
       </c>
       <c r="P79" s="46" t="s">
-        <v>455</v>
+        <v>463</v>
       </c>
       <c r="Q79" s="25"/>
       <c r="R79" s="26"/>
@@ -7950,13 +7947,13 @@
         <v>45428</v>
       </c>
       <c r="G102" s="24" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="H102" s="24" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="I102" s="24" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="J102" s="25" t="s">
         <v>84</v>

</xml_diff>